<commit_message>
trabajo escrito y graficas
</commit_message>
<xml_diff>
--- a/prototipo/muestras_tiempos/finales/muestras_tiempos_finales.xlsx
+++ b/prototipo/muestras_tiempos/finales/muestras_tiempos_finales.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\Desktop\tesis_ger\prototipo\muestras_tiempos\finales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB53E57-1DA6-4A20-A37E-BC93C4BED092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759997A4-7B57-4D0F-A9CC-A65D0F90A665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{80C2EF03-FE1F-48DB-B793-BDFDA14F5686}"/>
+    <workbookView xWindow="1950" yWindow="0" windowWidth="21600" windowHeight="15585" activeTab="1" xr2:uid="{80C2EF03-FE1F-48DB-B793-BDFDA14F5686}"/>
   </bookViews>
   <sheets>
     <sheet name="muestras_tiempos" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
   <si>
     <t>Agentes</t>
   </si>
@@ -558,7 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -571,6 +572,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -578,7 +582,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2327,8 +2331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FFD816-5BA1-4C19-8563-9BEDB4F63ECB}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,27 +2351,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2394,7 +2400,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -2406,11 +2412,11 @@
       <c r="D3" s="2">
         <v>0.36</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <f>AVERAGE(C3:C5)</f>
         <v>72.126666666666665</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <f>_xlfn.STDEV.S(C3:C5)</f>
         <v>1.9776777627645366</v>
       </c>
@@ -2420,17 +2426,17 @@
       <c r="H3" s="2">
         <v>133.715</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="7">
         <f>AVERAGE(G3:G5)</f>
         <v>70.98</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="7">
         <f>_xlfn.STDEV.S(G3:G5)</f>
         <v>2.4459981602609622</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -2440,19 +2446,19 @@
       <c r="D4" s="2">
         <v>0.38400000000000001</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="2">
         <v>69.353999999999999</v>
       </c>
       <c r="H4" s="2">
         <v>107.867</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -2462,19 +2468,19 @@
       <c r="D5" s="2">
         <v>0.36099999999999999</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="2">
         <v>73.793000000000006</v>
       </c>
       <c r="H5" s="2">
         <v>111.432</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
       <c r="B6" s="1">
@@ -2486,11 +2492,11 @@
       <c r="D6" s="2">
         <v>0.38600000000000001</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <f t="shared" ref="E6" si="0">AVERAGE(C6:C8)</f>
         <v>86.427000000000007</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <f t="shared" ref="F6" si="1">_xlfn.STDEV.S(C6:C8)</f>
         <v>6.79633437964908</v>
       </c>
@@ -2500,17 +2506,17 @@
       <c r="H6" s="2">
         <v>129.06800000000001</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="7">
         <f t="shared" ref="I6" si="2">AVERAGE(G6:G8)</f>
         <v>97.945000000000007</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="7">
         <f t="shared" ref="J6" si="3">_xlfn.STDEV.S(G6:G8)</f>
         <v>13.886285932530511</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -2520,19 +2526,19 @@
       <c r="D7" s="2">
         <v>0.39100000000000001</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="2">
         <v>92.816999999999993</v>
       </c>
       <c r="H7" s="2">
         <v>139.81</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -2542,19 +2548,19 @@
       <c r="D8" s="2">
         <v>0.39500000000000002</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="2">
         <v>87.352000000000004</v>
       </c>
       <c r="H8" s="2">
         <v>121.345</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>4</v>
       </c>
       <c r="B9" s="1">
@@ -2566,11 +2572,11 @@
       <c r="D9" s="2">
         <v>0.42799999999999999</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <f t="shared" ref="E9" si="4">AVERAGE(C9:C11)</f>
         <v>78.775999999999996</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="7">
         <f t="shared" ref="F9" si="5">_xlfn.STDEV.S(C9:C11)</f>
         <v>1.9301823748029621</v>
       </c>
@@ -2580,17 +2586,17 @@
       <c r="H9" s="2">
         <v>167.70699999999999</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="7">
         <f t="shared" ref="I9" si="6">AVERAGE(G9:G11)</f>
         <v>112.48066666666666</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="7">
         <f t="shared" ref="J9" si="7">_xlfn.STDEV.S(G9:G11)</f>
         <v>4.7548466151215978</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="1">
         <v>2</v>
       </c>
@@ -2600,19 +2606,19 @@
       <c r="D10" s="2">
         <v>0.439</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="2">
         <v>115.518</v>
       </c>
       <c r="H10" s="2">
         <v>168.31299999999999</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="1">
         <v>3</v>
       </c>
@@ -2622,19 +2628,19 @@
       <c r="D11" s="2">
         <v>0.441</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="2">
         <v>114.923</v>
       </c>
       <c r="H11" s="2">
         <v>160.48400000000001</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>5</v>
       </c>
       <c r="B12" s="1">
@@ -2646,11 +2652,11 @@
       <c r="D12" s="2">
         <v>0.504</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="7">
         <f t="shared" ref="E12" si="8">AVERAGE(C12:C14)</f>
         <v>143.22366666666667</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="7">
         <f t="shared" ref="F12" si="9">_xlfn.STDEV.S(C12:C14)</f>
         <v>44.050418412693134</v>
       </c>
@@ -2660,17 +2666,17 @@
       <c r="H12" s="2">
         <v>236.16900000000001</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="7">
         <f t="shared" ref="I12" si="10">AVERAGE(G12:G14)</f>
         <v>335.3776666666667</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="7">
         <f t="shared" ref="J12" si="11">_xlfn.STDEV.S(G12:G14)</f>
         <v>51.843885505749945</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -2680,19 +2686,19 @@
       <c r="D13" s="2">
         <v>0.504</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="2">
         <v>386.47699999999998</v>
       </c>
       <c r="H13" s="2">
         <v>282.40100000000001</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="1">
         <v>3</v>
       </c>
@@ -2702,32 +2708,21 @@
       <c r="D14" s="2">
         <v>0.503</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="2">
         <v>282.82</v>
       </c>
       <c r="H14" s="2">
         <v>226.39599999999999</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="C1:F1"/>
+  <mergeCells count="24">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="J3:J5"/>
     <mergeCell ref="J6:J8"/>
     <mergeCell ref="J9:J11"/>
@@ -2737,8 +2732,500 @@
     <mergeCell ref="I6:I8"/>
     <mergeCell ref="I9:I11"/>
     <mergeCell ref="I12:I14"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E12:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDD5BB0-C1D6-4A32-9235-30571F9B7796}">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="H1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>72.846000000000004</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="E3" s="7">
+        <f>AVERAGE(C3:C5)</f>
+        <v>72.126666666666665</v>
+      </c>
+      <c r="F3" s="7">
+        <f>_xlfn.STDEV.S(C3:C5)</f>
+        <v>1.9776777627645366</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>69.793000000000006</v>
+      </c>
+      <c r="K3" s="2">
+        <v>133.715</v>
+      </c>
+      <c r="L3" s="7">
+        <f>AVERAGE(J3:J5)</f>
+        <v>70.98</v>
+      </c>
+      <c r="M3" s="7">
+        <f>_xlfn.STDEV.S(J3:J5)</f>
+        <v>2.4459981602609622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>69.89</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>69.353999999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>107.867</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>73.644000000000005</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>73.793000000000006</v>
+      </c>
+      <c r="K5" s="2">
+        <v>111.432</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>82.828000000000003</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" ref="E6" si="0">AVERAGE(C6:C8)</f>
+        <v>86.427000000000007</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" ref="F6" si="1">_xlfn.STDEV.S(C6:C8)</f>
+        <v>6.79633437964908</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>113.666</v>
+      </c>
+      <c r="K6" s="2">
+        <v>129.06800000000001</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" ref="L6" si="2">AVERAGE(J6:J8)</f>
+        <v>97.945000000000007</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" ref="M6" si="3">_xlfn.STDEV.S(J6:J8)</f>
+        <v>13.886285932530511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>82.186999999999998</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>92.816999999999993</v>
+      </c>
+      <c r="K7" s="2">
+        <v>139.81</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>94.266000000000005</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="2">
+        <v>87.352000000000004</v>
+      </c>
+      <c r="K8" s="2">
+        <v>121.345</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>79.063999999999993</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" ref="E9" si="4">AVERAGE(C9:C11)</f>
+        <v>78.775999999999996</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" ref="F9" si="5">_xlfn.STDEV.S(C9:C11)</f>
+        <v>1.9301823748029621</v>
+      </c>
+      <c r="H9" s="6">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>107.001</v>
+      </c>
+      <c r="K9" s="2">
+        <v>167.70699999999999</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" ref="L9" si="6">AVERAGE(J9:J11)</f>
+        <v>112.48066666666666</v>
+      </c>
+      <c r="M9" s="7">
+        <f t="shared" ref="M9" si="7">_xlfn.STDEV.S(J9:J11)</f>
+        <v>4.7548466151215978</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>76.718000000000004</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.439</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>115.518</v>
+      </c>
+      <c r="K10" s="2">
+        <v>168.31299999999999</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>80.546000000000006</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.441</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="1">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>114.923</v>
+      </c>
+      <c r="K11" s="2">
+        <v>160.48400000000001</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>112.28</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.504</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" ref="E12" si="8">AVERAGE(C12:C14)</f>
+        <v>143.22366666666667</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" ref="F12" si="9">_xlfn.STDEV.S(C12:C14)</f>
+        <v>44.050418412693134</v>
+      </c>
+      <c r="H12" s="6">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>336.83600000000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>236.16900000000001</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" ref="L12" si="10">AVERAGE(J12:J14)</f>
+        <v>335.3776666666667</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" ref="M12" si="11">_xlfn.STDEV.S(J12:J14)</f>
+        <v>51.843885505749945</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>193.65700000000001</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.504</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>386.47699999999998</v>
+      </c>
+      <c r="K13" s="2">
+        <v>282.40100000000001</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>123.73399999999999</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.503</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="1">
+        <v>3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>282.82</v>
+      </c>
+      <c r="K14" s="2">
+        <v>226.39599999999999</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>